<commit_message>
Corrigindo resposta do ex aula 6 e upload aula 8
</commit_message>
<xml_diff>
--- a/Excel/Aula 6/Planilha_Exercícios.xlsx
+++ b/Excel/Aula 6/Planilha_Exercícios.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noteb\Desktop\Profissa\Material de Aula\Excel\Aula 6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48971D8-088F-48BE-8522-C78DFFBA2AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercício 1" sheetId="1" r:id="rId1"/>
     <sheet name="Exercício 2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -307,9 +313,6 @@
     <t>Beatriz de Lima Oliveira</t>
   </si>
   <si>
-    <t>Qual o endereço do funcionário de nome Adelino Werneck?</t>
-  </si>
-  <si>
     <t>Qual a data de nascimento do funcionário de ID 334?</t>
   </si>
   <si>
@@ -317,19 +320,22 @@
 </t>
   </si>
   <si>
-    <t>Qual o sexo do funcionário de nome Ana Barbosa?</t>
-  </si>
-  <si>
     <t>Qual o sexo do entrevistado número 13?</t>
   </si>
   <si>
     <t>Qual a faixa etária do entrevistado numero 48?</t>
+  </si>
+  <si>
+    <t>Qual o endereço do funcionário de ID 291?</t>
+  </si>
+  <si>
+    <t>Qual o estado civíl do funcionário de ID486</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,8 +387,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -405,15 +417,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,12 +460,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,44 +503,47 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela3" displayName="Tabela3" ref="A1:F66" totalsRowShown="0">
-  <autoFilter ref="A1:F66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela3" displayName="Tabela3" ref="A1:F66" totalsRowShown="0">
+  <autoFilter ref="A1:F66" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Entrevistado"/>
-    <tableColumn id="2" name="Religião"/>
-    <tableColumn id="3" name="Sexo"/>
-    <tableColumn id="4" name="Faixa etária"/>
-    <tableColumn id="5" name="Região do país"/>
-    <tableColumn id="6" name="Voto"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Entrevistado"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Religião"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sexo"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Faixa etária"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Região do país"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Voto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F50" totalsRowShown="0">
-  <autoFilter ref="A1:F50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela2" displayName="Tabela2" ref="A1:F50" totalsRowShown="0">
+  <autoFilter ref="A1:F50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID RH"/>
-    <tableColumn id="2" name="Nome Completo"/>
-    <tableColumn id="3" name="Estado Civil"/>
-    <tableColumn id="4" name="Sexo"/>
-    <tableColumn id="5" name="Data de Nascimento" dataDxfId="0"/>
-    <tableColumn id="6" name="Endereço"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID RH"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Nome Completo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Estado Civil"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Sexo"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Data de Nascimento" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Endereço"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -518,7 +581,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -590,7 +653,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -763,23 +826,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,18 +861,18 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
       <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -828,16 +891,16 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -856,16 +919,16 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -884,16 +947,16 @@
       <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="H4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -912,16 +975,16 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="H5" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -941,7 +1004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -961,7 +1024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -981,7 +1044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1001,7 +1064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1021,7 +1084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1041,7 +1104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1061,7 +1124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1081,7 +1144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1101,7 +1164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1121,7 +1184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1141,7 +1204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1161,7 +1224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1181,7 +1244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1201,7 +1264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1221,7 +1284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1241,7 +1304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1261,7 +1324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1281,7 +1344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1301,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1321,7 +1384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1341,7 +1404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1361,7 +1424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1381,7 +1444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1401,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1421,7 +1484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1441,7 +1504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1461,7 +1524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1481,7 +1544,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1501,7 +1564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1521,7 +1584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1541,7 +1604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1561,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1581,7 +1644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1601,7 +1664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1621,7 +1684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1641,7 +1704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1661,7 +1724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1681,7 +1744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1701,7 +1764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1721,7 +1784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1741,7 +1804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1761,7 +1824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1781,7 +1844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1801,7 +1864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1821,7 +1884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1841,7 +1904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1861,7 +1924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1881,7 +1944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1901,7 +1964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1921,7 +1984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1941,7 +2004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1961,7 +2024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1981,7 +2044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2001,7 +2064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2021,7 +2084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2041,7 +2104,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2061,7 +2124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2081,7 +2144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2101,7 +2164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2121,7 +2184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2150,7 +2213,7 @@
     <mergeCell ref="H5:L5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D66">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"menor que 30 anos,entre 30 e 50 anos,maior que 50 anos"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2162,1072 +2225,1127 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="73.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>460</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="4">
         <v>28007</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="H2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>27118</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>195</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4">
+        <v>35547</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>195</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4">
+        <v>34312</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="4">
+        <v>28080</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="8">
-        <v>35547</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E7" s="4">
+        <v>29378</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="4">
+        <v>27644</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>342</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4">
+        <v>31638</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>320</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4">
+        <v>27933</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="4">
+        <v>29833</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="4">
+        <v>29815</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>291</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="4">
+        <v>33931</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="4">
+        <v>36339</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>425</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4">
+        <v>30369</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4">
+        <v>32880</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>217</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="4">
+        <v>32627</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="4">
+        <v>30820</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>240</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="4">
+        <v>33384</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>435</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="4">
+        <v>31204</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>405</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4">
+        <v>29468</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>209</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="4">
+        <v>35823</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>334</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4">
+        <v>36144</v>
+      </c>
+      <c r="F23" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>102</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>448</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="4">
+        <v>27693</v>
+      </c>
+      <c r="F24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>354</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="4">
+        <v>26592</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>375</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="4">
+        <v>29583</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>237</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="4">
+        <v>29084</v>
+      </c>
+      <c r="F27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>363</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="8">
-        <v>34312</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E28" s="4">
+        <v>29619</v>
+      </c>
+      <c r="F28" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>133</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="4">
+        <v>32690</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>469</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="4">
+        <v>33693</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>147</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="4">
+        <v>31458</v>
+      </c>
+      <c r="F31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="4">
+        <v>26528</v>
+      </c>
+      <c r="F32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>287</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="4">
+        <v>35916</v>
+      </c>
+      <c r="F33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>286</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="8">
-        <v>28080</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E34" s="4">
+        <v>29515</v>
+      </c>
+      <c r="F34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>151</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="4">
+        <v>27645</v>
+      </c>
+      <c r="F35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="4">
+        <v>35119</v>
+      </c>
+      <c r="F36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>537</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="4">
+        <v>34170</v>
+      </c>
+      <c r="F37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>271</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="4">
+        <v>26108</v>
+      </c>
+      <c r="F38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>457</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="4">
+        <v>30588</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>371</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="4">
+        <v>35630</v>
+      </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>316</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="4">
+        <v>31773</v>
+      </c>
+      <c r="F41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>218</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="4">
+        <v>25579</v>
+      </c>
+      <c r="F42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="4">
+        <v>31088</v>
+      </c>
+      <c r="F43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="4">
+        <v>36299</v>
+      </c>
+      <c r="F44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>343</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="4">
+        <v>32174</v>
+      </c>
+      <c r="F45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>499</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="4">
+        <v>33866</v>
+      </c>
+      <c r="F46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>370</v>
+      </c>
+      <c r="B47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="C47" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="8">
-        <v>29378</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="4">
+        <v>36233</v>
+      </c>
+      <c r="F47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="4">
+        <v>35703</v>
+      </c>
+      <c r="F48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>455</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="4">
+        <v>32281</v>
+      </c>
+      <c r="F49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>486</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" s="4">
+        <v>30614</v>
+      </c>
+      <c r="F50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>167</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="8">
-        <v>27644</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>342</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="8">
-        <v>31638</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>320</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="8">
-        <v>27933</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>88</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="8">
-        <v>29833</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>113</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="8">
-        <v>29815</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>291</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="8">
-        <v>33931</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>95</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="8">
-        <v>36339</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>425</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="8">
-        <v>30369</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>3</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="8">
-        <v>32880</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>217</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="8">
-        <v>32627</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>158</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="8">
-        <v>30820</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>240</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="8">
-        <v>33384</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>435</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="8">
-        <v>31204</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>405</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="8">
-        <v>29468</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>209</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="8">
-        <v>35823</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>334</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="8">
-        <v>36144</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
-        <v>448</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="8">
-        <v>27693</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>354</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="8">
-        <v>26592</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>375</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="8">
-        <v>29583</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>237</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="8">
-        <v>29084</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
-        <v>363</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="8">
-        <v>29619</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
-        <v>10</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="8">
-        <v>32690</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>469</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="8">
-        <v>33693</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>147</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="8">
-        <v>31458</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>11</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="8">
-        <v>26528</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
-        <v>287</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="8">
-        <v>35916</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>286</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="8">
-        <v>29515</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>151</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="8">
-        <v>27645</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
-        <v>145</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="8">
-        <v>35119</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
-        <v>537</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="8">
-        <v>34170</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
-        <v>271</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E38" s="8">
-        <v>26108</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
-        <v>457</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="8">
-        <v>30588</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
-        <v>371</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="8">
-        <v>35630</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
-        <v>316</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="8">
-        <v>31773</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
-        <v>218</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="8">
-        <v>25579</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
-        <v>74</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E43" s="8">
-        <v>31088</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
-        <v>6</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" s="8">
-        <v>36299</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
-        <v>343</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="8">
-        <v>32174</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
-        <v>499</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="8">
-        <v>33866</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>370</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="8">
-        <v>36233</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
-        <v>23</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="8">
-        <v>35703</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
-        <v>455</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" s="8">
-        <v>32281</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
-        <v>486</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E50" s="8">
-        <v>30614</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="H5:L5"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3238,12 +3356,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>